<commit_message>
More data analysis on mode 2
</commit_message>
<xml_diff>
--- a/Location Logger/kml_converter_template.xlsx
+++ b/Location Logger/kml_converter_template.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Location" localSheetId="0">Sheet1!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -16,6 +19,21 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="Location.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" firstRow="2" sourceFile="Macintosh HD:Users:atitus:GreekEasy:Location Logger:3_27_data_2:Location.csv" tab="0" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,12 +420,15 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>